<commit_message>
direction discrimination with two staircases
</commit_message>
<xml_diff>
--- a/07-motion-direction/2d-motion-direction-discrimination/staircase_parameters.xlsx
+++ b/07-motion-direction/2d-motion-direction-discrimination/staircase_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/kbonnen_iu_edu/Documents/Courses/V768-Measuring-Perception/V768-Psychophysics-labs/05-adaptive-methods/adaptive-methods/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/kbonnen_iu_edu/Documents/Courses/V768-Measuring-Perception/V768-Psychophysics-labs/07-motion-direction/2d-motion-direction-discrimination/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{44A74B6C-5AB4-1D45-9146-C88ED770F71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1C5A302-9365-B448-BA2B-C8E15AB3298D}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="8_{44A74B6C-5AB4-1D45-9146-C88ED770F71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABA1944C-6782-9F4C-8B82-463853164BB7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25780" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -55,12 +55,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-The label given to this staircase.</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The label given to this staircase.</t>
         </r>
       </text>
     </comment>
@@ -316,7 +325,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>label</t>
   </si>
@@ -363,7 +372,7 @@
     <t>lo</t>
   </si>
   <si>
-    <t>[2,.5]</t>
+    <t>base_direction</t>
   </si>
 </sst>
 </file>
@@ -788,11 +797,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -801,7 +810,7 @@
     <col min="2" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -832,25 +841,28 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
+      <c r="F2">
+        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -861,25 +873,28 @@
       <c r="I2">
         <v>2</v>
       </c>
+      <c r="K2">
+        <v>45</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>-10</v>
+        <v>-14</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
+        <v>-20</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -890,8 +905,11 @@
       <c r="I3">
         <v>1</v>
       </c>
+      <c r="K3">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -899,13 +917,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -922,8 +940,11 @@
       <c r="J4">
         <v>0</v>
       </c>
+      <c r="K4">
+        <v>45</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -931,13 +952,13 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="D5">
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="E5">
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -953,6 +974,143 @@
       </c>
       <c r="J5">
         <v>0</v>
+      </c>
+      <c r="K5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>-14</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>-20</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>-14</v>
+      </c>
+      <c r="D9">
+        <v>-20</v>
+      </c>
+      <c r="E9">
+        <v>-20</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -968,18 +1126,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1097,24 +1255,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>